<commit_message>
test commit on branch
</commit_message>
<xml_diff>
--- a/TestFolder/test.xlsx
+++ b/TestFolder/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,38 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>te</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>testw</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -53,7 +77,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -69,7 +93,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +138,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +173,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,12 +355,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>